<commit_message>
[FIX] PROD mode ativado
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_eShare\PROD\dhl-dtentry-sharepoint-migration\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A47D64-A2B5-42DF-9755-7E00FD289AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9ADC4C0-2AF7-4F13-9F7C-E96D0DD122D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
     <t>C:\Users\##USERNAME##\DPDHL\PtP Brasil - PAGAMENTOS DE EXCEÇÕES\01 - TESTE ROBOTIZAÇÃO - DATA ENTRY\HOMOLOGAÇÃO</t>
   </si>
   <si>
-    <t>QA-PPD</t>
-  </si>
-  <si>
     <t>Isaque.M.Vieira@dhl.com</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -898,7 +898,7 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
         <v>78</v>
@@ -2000,7 +2000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -2259,7 +2259,7 @@
         <v>91</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
[FIX] Ajuste no Config: caminho do Drive estava errado
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_eShare\PROD\dhl-dtentry-sharepoint-migration\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9ADC4C0-2AF7-4F13-9F7C-E96D0DD122D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BC9F63-F97E-4F8E-91D2-CB3736FC7044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -909,11 +909,11 @@
       <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="D19" t="s">
         <v>67</v>
@@ -924,11 +924,11 @@
       <c r="A21" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="C21" t="s">
-        <v>108</v>
       </c>
       <c r="D21" t="s">
         <v>98</v>
@@ -938,11 +938,11 @@
       <c r="A22" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="C22" t="s">
-        <v>109</v>
       </c>
       <c r="D22" t="s">
         <v>64</v>
@@ -952,11 +952,11 @@
       <c r="A23" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="C23" t="s">
-        <v>110</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -1011,11 +1011,11 @@
       <c r="A34" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>